<commit_message>
Fixed right clicked empty table. reformatted FileSubmitter
</commit_message>
<xml_diff>
--- a/plyj-master/Test.xlsx
+++ b/plyj-master/Test.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
   <si>
     <t>id</t>
   </si>
@@ -25,6 +25,12 @@
     <t>timestamp</t>
   </si>
   <si>
+    <t>datasize</t>
+  </si>
+  <si>
+    <t>DateAnalyzed</t>
+  </si>
+  <si>
     <t>ESLOC</t>
   </si>
   <si>
@@ -158,72 +164,6 @@
   </si>
   <si>
     <t>LocalizationOfVar</t>
-  </si>
-  <si>
-    <t>Test</t>
-  </si>
-  <si>
-    <t>Hello</t>
-  </si>
-  <si>
-    <t>13</t>
-  </si>
-  <si>
-    <t>28</t>
-  </si>
-  <si>
-    <t>29</t>
-  </si>
-  <si>
-    <t>30</t>
-  </si>
-  <si>
-    <t>31</t>
-  </si>
-  <si>
-    <t>32</t>
-  </si>
-  <si>
-    <t>33</t>
-  </si>
-  <si>
-    <t>34</t>
-  </si>
-  <si>
-    <t>35</t>
-  </si>
-  <si>
-    <t>36</t>
-  </si>
-  <si>
-    <t>37</t>
-  </si>
-  <si>
-    <t>38</t>
-  </si>
-  <si>
-    <t>39</t>
-  </si>
-  <si>
-    <t>40</t>
-  </si>
-  <si>
-    <t>41</t>
-  </si>
-  <si>
-    <t>42</t>
-  </si>
-  <si>
-    <t>43</t>
-  </si>
-  <si>
-    <t>44</t>
-  </si>
-  <si>
-    <t>45</t>
-  </si>
-  <si>
-    <t>Java</t>
   </si>
 </sst>
 </file>
@@ -564,16 +504,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AV4"/>
+  <dimension ref="A1:AX1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="51" width="20.7109375" customWidth="1"/>
+    <col min="2" max="76" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:48">
+    <row r="1" spans="1:50">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -718,443 +658,11 @@
       <c r="AV1" s="1" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="2" spans="1:48">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="AW1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="C2" t="s">
+      <c r="AX1" s="1" t="s">
         <v>49</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2">
-        <v>2</v>
-      </c>
-      <c r="F2">
-        <v>3</v>
-      </c>
-      <c r="G2">
-        <v>4</v>
-      </c>
-      <c r="H2">
-        <v>5</v>
-      </c>
-      <c r="I2">
-        <v>6</v>
-      </c>
-      <c r="J2">
-        <v>7</v>
-      </c>
-      <c r="K2">
-        <v>8</v>
-      </c>
-      <c r="L2">
-        <v>9</v>
-      </c>
-      <c r="M2">
-        <v>10</v>
-      </c>
-      <c r="N2">
-        <v>11</v>
-      </c>
-      <c r="O2">
-        <v>12</v>
-      </c>
-      <c r="P2" t="s">
-        <v>50</v>
-      </c>
-      <c r="Q2">
-        <v>14</v>
-      </c>
-      <c r="R2">
-        <v>15</v>
-      </c>
-      <c r="S2">
-        <v>16</v>
-      </c>
-      <c r="T2">
-        <v>17</v>
-      </c>
-      <c r="U2">
-        <v>18</v>
-      </c>
-      <c r="V2">
-        <v>19</v>
-      </c>
-      <c r="W2">
-        <v>20</v>
-      </c>
-      <c r="X2">
-        <v>21</v>
-      </c>
-      <c r="Y2">
-        <v>22</v>
-      </c>
-      <c r="Z2">
-        <v>23</v>
-      </c>
-      <c r="AA2">
-        <v>24</v>
-      </c>
-      <c r="AB2">
-        <v>25</v>
-      </c>
-      <c r="AC2">
-        <v>26</v>
-      </c>
-      <c r="AD2">
-        <v>27</v>
-      </c>
-      <c r="AE2" t="s">
-        <v>51</v>
-      </c>
-      <c r="AF2" t="s">
-        <v>52</v>
-      </c>
-      <c r="AG2" t="s">
-        <v>53</v>
-      </c>
-      <c r="AH2" t="s">
-        <v>54</v>
-      </c>
-      <c r="AI2" t="s">
-        <v>55</v>
-      </c>
-      <c r="AJ2" t="s">
-        <v>56</v>
-      </c>
-      <c r="AK2" t="s">
-        <v>57</v>
-      </c>
-      <c r="AL2" t="s">
-        <v>58</v>
-      </c>
-      <c r="AM2" t="s">
-        <v>59</v>
-      </c>
-      <c r="AN2" t="s">
-        <v>60</v>
-      </c>
-      <c r="AO2" t="s">
-        <v>61</v>
-      </c>
-      <c r="AP2" t="s">
-        <v>62</v>
-      </c>
-      <c r="AQ2" t="s">
-        <v>63</v>
-      </c>
-      <c r="AR2" t="s">
-        <v>64</v>
-      </c>
-      <c r="AS2" t="s">
-        <v>65</v>
-      </c>
-      <c r="AT2" t="s">
-        <v>66</v>
-      </c>
-      <c r="AU2" t="s">
-        <v>67</v>
-      </c>
-      <c r="AV2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="3" spans="1:48">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>49</v>
-      </c>
-      <c r="C3" t="s">
-        <v>49</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-      <c r="E3">
-        <v>2</v>
-      </c>
-      <c r="F3">
-        <v>3</v>
-      </c>
-      <c r="G3">
-        <v>4</v>
-      </c>
-      <c r="H3">
-        <v>5</v>
-      </c>
-      <c r="I3">
-        <v>6</v>
-      </c>
-      <c r="J3">
-        <v>7</v>
-      </c>
-      <c r="K3">
-        <v>8</v>
-      </c>
-      <c r="L3">
-        <v>9</v>
-      </c>
-      <c r="M3">
-        <v>10</v>
-      </c>
-      <c r="N3">
-        <v>11</v>
-      </c>
-      <c r="O3">
-        <v>12</v>
-      </c>
-      <c r="P3" t="s">
-        <v>50</v>
-      </c>
-      <c r="Q3">
-        <v>14</v>
-      </c>
-      <c r="R3">
-        <v>15</v>
-      </c>
-      <c r="S3">
-        <v>16</v>
-      </c>
-      <c r="T3">
-        <v>17</v>
-      </c>
-      <c r="U3">
-        <v>18</v>
-      </c>
-      <c r="V3">
-        <v>19</v>
-      </c>
-      <c r="W3">
-        <v>20</v>
-      </c>
-      <c r="X3">
-        <v>21</v>
-      </c>
-      <c r="Y3">
-        <v>22</v>
-      </c>
-      <c r="Z3">
-        <v>23</v>
-      </c>
-      <c r="AA3">
-        <v>24</v>
-      </c>
-      <c r="AB3">
-        <v>25</v>
-      </c>
-      <c r="AC3">
-        <v>26</v>
-      </c>
-      <c r="AD3">
-        <v>27</v>
-      </c>
-      <c r="AE3" t="s">
-        <v>51</v>
-      </c>
-      <c r="AF3" t="s">
-        <v>52</v>
-      </c>
-      <c r="AG3" t="s">
-        <v>53</v>
-      </c>
-      <c r="AH3" t="s">
-        <v>54</v>
-      </c>
-      <c r="AI3" t="s">
-        <v>55</v>
-      </c>
-      <c r="AJ3" t="s">
-        <v>56</v>
-      </c>
-      <c r="AK3" t="s">
-        <v>57</v>
-      </c>
-      <c r="AL3" t="s">
-        <v>58</v>
-      </c>
-      <c r="AM3" t="s">
-        <v>59</v>
-      </c>
-      <c r="AN3" t="s">
-        <v>60</v>
-      </c>
-      <c r="AO3" t="s">
-        <v>61</v>
-      </c>
-      <c r="AP3" t="s">
-        <v>62</v>
-      </c>
-      <c r="AQ3" t="s">
-        <v>63</v>
-      </c>
-      <c r="AR3" t="s">
-        <v>64</v>
-      </c>
-      <c r="AS3" t="s">
-        <v>65</v>
-      </c>
-      <c r="AT3" t="s">
-        <v>66</v>
-      </c>
-      <c r="AU3" t="s">
-        <v>67</v>
-      </c>
-      <c r="AV3" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="4" spans="1:48">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>69</v>
-      </c>
-      <c r="C4" t="s">
-        <v>49</v>
-      </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
-      <c r="E4">
-        <v>2</v>
-      </c>
-      <c r="F4">
-        <v>3</v>
-      </c>
-      <c r="G4">
-        <v>4</v>
-      </c>
-      <c r="H4">
-        <v>5</v>
-      </c>
-      <c r="I4">
-        <v>6</v>
-      </c>
-      <c r="J4">
-        <v>7</v>
-      </c>
-      <c r="K4">
-        <v>8</v>
-      </c>
-      <c r="L4">
-        <v>9</v>
-      </c>
-      <c r="M4">
-        <v>10</v>
-      </c>
-      <c r="N4">
-        <v>11</v>
-      </c>
-      <c r="O4">
-        <v>12</v>
-      </c>
-      <c r="P4" t="s">
-        <v>50</v>
-      </c>
-      <c r="Q4">
-        <v>14</v>
-      </c>
-      <c r="R4">
-        <v>15</v>
-      </c>
-      <c r="S4">
-        <v>16</v>
-      </c>
-      <c r="T4">
-        <v>17</v>
-      </c>
-      <c r="U4">
-        <v>18</v>
-      </c>
-      <c r="V4">
-        <v>19</v>
-      </c>
-      <c r="W4">
-        <v>20</v>
-      </c>
-      <c r="X4">
-        <v>21</v>
-      </c>
-      <c r="Y4">
-        <v>22</v>
-      </c>
-      <c r="Z4">
-        <v>23</v>
-      </c>
-      <c r="AA4">
-        <v>24</v>
-      </c>
-      <c r="AB4">
-        <v>25</v>
-      </c>
-      <c r="AC4">
-        <v>26</v>
-      </c>
-      <c r="AD4">
-        <v>27</v>
-      </c>
-      <c r="AE4" t="s">
-        <v>51</v>
-      </c>
-      <c r="AF4" t="s">
-        <v>52</v>
-      </c>
-      <c r="AG4" t="s">
-        <v>53</v>
-      </c>
-      <c r="AH4" t="s">
-        <v>54</v>
-      </c>
-      <c r="AI4" t="s">
-        <v>55</v>
-      </c>
-      <c r="AJ4" t="s">
-        <v>56</v>
-      </c>
-      <c r="AK4" t="s">
-        <v>57</v>
-      </c>
-      <c r="AL4" t="s">
-        <v>58</v>
-      </c>
-      <c r="AM4" t="s">
-        <v>59</v>
-      </c>
-      <c r="AN4" t="s">
-        <v>60</v>
-      </c>
-      <c r="AO4" t="s">
-        <v>61</v>
-      </c>
-      <c r="AP4" t="s">
-        <v>62</v>
-      </c>
-      <c r="AQ4" t="s">
-        <v>63</v>
-      </c>
-      <c r="AR4" t="s">
-        <v>64</v>
-      </c>
-      <c r="AS4" t="s">
-        <v>65</v>
-      </c>
-      <c r="AT4" t="s">
-        <v>66</v>
-      </c>
-      <c r="AU4" t="s">
-        <v>67</v>
-      </c>
-      <c r="AV4" t="s">
-        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>